<commit_message>
Add swift sneak enchantment
</commit_message>
<xml_diff>
--- a/scripts/Enchantment Details.xlsx
+++ b/scripts/Enchantment Details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
   <si>
     <t xml:space="preserve">Enchantment</t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t xml:space="preserve">Increases sweep attack damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swift_sneak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increases speed while sneaking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leggings</t>
   </si>
   <si>
     <t xml:space="preserve">thorns</t>
@@ -380,9 +389,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Description" displayName="Description" ref="B:B" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Description" displayName="Description" ref="A1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" name="Description"/>
+    <tableColumn id="1" name="Enchantment"/>
   </tableColumns>
 </table>
 </file>
@@ -395,7 +404,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -810,32 +819,42 @@
         <v>84</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
New descriptions, fixes spelling
</commit_message>
<xml_diff>
--- a/scripts/Enchantment Details.xlsx
+++ b/scripts/Enchantment Details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
   <si>
     <t xml:space="preserve">Enchantment</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">aqua_affinity</t>
   </si>
   <si>
-    <t xml:space="preserve">Speeds up mining underwater</t>
+    <t xml:space="preserve">Increases mining speed while underwater</t>
   </si>
   <si>
     <t xml:space="preserve">Helmets</t>
@@ -46,73 +46,76 @@
     <t xml:space="preserve">Increases damage dealt to arthropods</t>
   </si>
   <si>
+    <t xml:space="preserve">Melee Weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binding_curse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makes the wearer unable to remove the armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blast_protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduces damage taken from explosions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strikes lightning when thrown in a thunderstorm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tridents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depth_strider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increases swimming speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increases mining speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feather_falling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduces fall damage taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fire_aspect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets the target on fire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Swords</t>
   </si>
   <si>
-    <t xml:space="preserve">binding_curse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Makes the wearer unable to take off the armor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blast_protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reduces taken explosion damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">channeling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strikes lightning during storms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tridents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">depth_strider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Makes the wearer swim faster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increases mining speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feather_falling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reduces fall damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fire_aspect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lights targets on fire</t>
-  </si>
-  <si>
     <t xml:space="preserve">fire_protection</t>
   </si>
   <si>
-    <t xml:space="preserve">Reduces taken fire damage</t>
+    <t xml:space="preserve">Reduces damage taken from fire</t>
   </si>
   <si>
     <t xml:space="preserve">flame</t>
   </si>
   <si>
-    <t xml:space="preserve">Lights arrows on fire</t>
+    <t xml:space="preserve">Sets shot arrows on fire</t>
   </si>
   <si>
     <t xml:space="preserve">Bows</t>
@@ -121,13 +124,13 @@
     <t xml:space="preserve">fortune</t>
   </si>
   <si>
-    <t xml:space="preserve">Increases drop rates from ores</t>
+    <t xml:space="preserve">Increases drop amount from some blocks</t>
   </si>
   <si>
     <t xml:space="preserve">frost_walker</t>
   </si>
   <si>
-    <t xml:space="preserve">Creates ice when walking on water</t>
+    <t xml:space="preserve">Creates an ice path when walking on water</t>
   </si>
   <si>
     <t xml:space="preserve">impaling</t>
@@ -139,7 +142,7 @@
     <t xml:space="preserve">infinity</t>
   </si>
   <si>
-    <t xml:space="preserve">Stops the bow from consuming arrows</t>
+    <t xml:space="preserve">Prevents arrows from being consumed when shot</t>
   </si>
   <si>
     <t xml:space="preserve">knockback</t>
@@ -151,13 +154,13 @@
     <t xml:space="preserve">looting</t>
   </si>
   <si>
-    <t xml:space="preserve">Increases loot drops from mobs</t>
+    <t xml:space="preserve">Increases amount of loot dropped by mobs</t>
   </si>
   <si>
     <t xml:space="preserve">loyalty</t>
   </si>
   <si>
-    <t xml:space="preserve">Returns trident to thrower</t>
+    <t xml:space="preserve">Returns trident to thrower after it is thrown</t>
   </si>
   <si>
     <t xml:space="preserve">luck_of_the_sea</t>
@@ -187,7 +190,7 @@
     <t xml:space="preserve">multishot</t>
   </si>
   <si>
-    <t xml:space="preserve">Shoots multiple arrows</t>
+    <t xml:space="preserve">Shoots three projectiles at once</t>
   </si>
   <si>
     <t xml:space="preserve">Crossbows</t>
@@ -196,13 +199,13 @@
     <t xml:space="preserve">piercing</t>
   </si>
   <si>
-    <t xml:space="preserve">Arrows can pierce through targets and shields</t>
+    <t xml:space="preserve">Allows arrows to pierce through targets and shields</t>
   </si>
   <si>
     <t xml:space="preserve">power</t>
   </si>
   <si>
-    <t xml:space="preserve">Increases damage dealt </t>
+    <t xml:space="preserve">Increases damage dealt with arrows</t>
   </si>
   <si>
     <t xml:space="preserve">projectile_protection</t>
@@ -220,10 +223,13 @@
     <t xml:space="preserve">punch</t>
   </si>
   <si>
+    <t xml:space="preserve">Increases knockback dealt with arrows</t>
+  </si>
+  <si>
     <t xml:space="preserve">quick_charge</t>
   </si>
   <si>
-    <t xml:space="preserve">Reloads arrows quicker</t>
+    <t xml:space="preserve">Reloads the crossbow quicker</t>
   </si>
   <si>
     <t xml:space="preserve">respiration</t>
@@ -235,16 +241,13 @@
     <t xml:space="preserve">riptide</t>
   </si>
   <si>
-    <t xml:space="preserve">Launches the user when thrown in water</t>
+    <t xml:space="preserve">Launches the user when used in water</t>
   </si>
   <si>
     <t xml:space="preserve">sharpness</t>
   </si>
   <si>
-    <t xml:space="preserve">Increases damage dealt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melee Weapons</t>
+    <t xml:space="preserve">Increases damage dealt to everything</t>
   </si>
   <si>
     <t xml:space="preserve">silk_touch</t>
@@ -256,13 +259,13 @@
     <t xml:space="preserve">smite</t>
   </si>
   <si>
-    <t xml:space="preserve">Increases damage dealt to undead</t>
+    <t xml:space="preserve">Increases damage dealt to undead tagets</t>
   </si>
   <si>
     <t xml:space="preserve">soul_speed</t>
   </si>
   <si>
-    <t xml:space="preserve">The wearer walks faster on soul blocks</t>
+    <t xml:space="preserve">Increases movement speed on soul blocks</t>
   </si>
   <si>
     <t xml:space="preserve">sweeping_edge</t>
@@ -283,7 +286,7 @@
     <t xml:space="preserve">thorns</t>
   </si>
   <si>
-    <t xml:space="preserve">Damages melee attackers of the wearer</t>
+    <t xml:space="preserve">Deals damage to those who attack the wearer</t>
   </si>
   <si>
     <t xml:space="preserve">unbreaking</t>
@@ -404,7 +407,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,15 +525,15 @@
         <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>11</v>
@@ -538,21 +541,21 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>22</v>
@@ -560,10 +563,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>19</v>
@@ -571,10 +574,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>16</v>
@@ -582,43 +585,43 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>16</v>
@@ -626,76 +629,76 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>11</v>
@@ -703,10 +706,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>11</v>
@@ -714,32 +717,32 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>5</v>
@@ -747,10 +750,10 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>16</v>
@@ -758,21 +761,21 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>22</v>
@@ -780,21 +783,21 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>19</v>
@@ -802,32 +805,32 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>11</v>
@@ -835,24 +838,24 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix sweeping edge not updating description
</commit_message>
<xml_diff>
--- a/scripts/Enchantment Details.xlsx
+++ b/scripts/Enchantment Details.xlsx
@@ -268,7 +268,7 @@
     <t xml:space="preserve">Increases movement speed on soul blocks</t>
   </si>
   <si>
-    <t xml:space="preserve">sweeping_edge</t>
+    <t xml:space="preserve">sweeping</t>
   </si>
   <si>
     <t xml:space="preserve">Increases sweep attack damage</t>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>